<commit_message>
update bao cao lân 2
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\GitHub\Congnghephanmem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE65608F-B93A-4A09-A9DA-A9C57215FF78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8520"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Công việc</t>
   </si>
@@ -105,7 +111,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,6 +152,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -194,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,9 +236,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,6 +288,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -437,11 +480,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +493,7 @@
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -461,46 +504,43 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="F4">
+      <c r="E4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="F5">
+      <c r="E5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -510,11 +550,11 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="F6">
+      <c r="E6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -524,11 +564,11 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="F7">
+      <c r="E7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -538,11 +578,11 @@
       <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="F8">
+      <c r="E8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -552,11 +592,11 @@
       <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="F9">
+      <c r="E9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -566,11 +606,11 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="F10">
+      <c r="E10">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -580,11 +620,11 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="F11">
+      <c r="E11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -594,11 +634,11 @@
       <c r="D12" t="s">
         <v>27</v>
       </c>
-      <c r="F12">
+      <c r="E12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -608,7 +648,7 @@
       <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="F13">
+      <c r="E13">
         <v>3</v>
       </c>
     </row>
@@ -618,7 +658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -630,7 +670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>